<commit_message>
Changed gap in attachment hook to 4.1mm
The part on the attachments that looks like an arrow has a gap o 4.1mm
</commit_message>
<xml_diff>
--- a/Flower bots/Lily/BOMLily.xlsx
+++ b/Flower bots/Lily/BOMLily.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcena\Documents\GitHub\Lily-Bot\Flower bots\Lily\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B6690B-0BCC-4CA4-8F9F-E3A18B76AE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D3DB50-1C6C-4D9F-BF22-8454AD2DFCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0EC8DD03-4D44-45E9-BA35-044F8A99C324}"/>
   </bookViews>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Link</t>
   </si>
@@ -53,56 +47,107 @@
     <t>Price total</t>
   </si>
   <si>
-    <t>Mini breadborads</t>
-  </si>
-  <si>
-    <t>wheels</t>
-  </si>
-  <si>
-    <t>motors</t>
-  </si>
-  <si>
-    <t>Motor drivers</t>
-  </si>
-  <si>
-    <t>10mm screw</t>
-  </si>
-  <si>
-    <t>25mm screws</t>
-  </si>
-  <si>
-    <t>6mm screws</t>
-  </si>
-  <si>
-    <t>Uno chip</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/ZRM-Battery-5-5x2-1-Connector-Arduino/dp/B08P1L6JQT/ref=sr_1_4?crid=19WCGTTEUOR6V&amp;keywords=battery+holder+4xAA+male+connector&amp;qid=1668033662&amp;s=electronics&amp;sprefix=battery+holder+4xaa+male+connector%2Celectronics%2C117&amp;sr=1-4</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/DaFuRui-tie-Points-Solderless-Breadboard-Compatible/dp/B07KGQ7H8B/ref=sr_1_1_sspa?crid=37B9YN3ZDB607&amp;keywords=mini+breadboard&amp;qid=1668033762&amp;s=electronics&amp;sprefix=mini+bread%2Celectronics%2C112&amp;sr=1-1-spons&amp;psc=1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/AEDIKO-Motor-Gearbox-Shaft-200RPM/dp/B099Z85573/ref=sr_1_5?crid=1FLS6AZQIX9VS&amp;keywords=wheels+dc+motor&amp;qid=1668033941&amp;sprefix=wheels+dc+motor%2Caps%2C170&amp;sr=8-5</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/2448</t>
-  </si>
-  <si>
-    <t>Battery pack 9V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batteries AA (1.5V) </t>
+    <t>Upper Chassis </t>
+  </si>
+  <si>
+    <t>Lower Chassis </t>
+  </si>
+  <si>
+    <t>Standoffs </t>
+  </si>
+  <si>
+    <t>TB6612 Motor Driver </t>
+  </si>
+  <si>
+    <t>Arduino Uno </t>
+  </si>
+  <si>
+    <t>Mini Breadboard </t>
+  </si>
+  <si>
+    <t>Motor Mounts </t>
+  </si>
+  <si>
+    <t>Toy Motors </t>
+  </si>
+  <si>
+    <t>Toy Tire Wheels </t>
+  </si>
+  <si>
+    <t>5AA Battery Holder </t>
+  </si>
+  <si>
+    <t>Cinch strap </t>
+  </si>
+  <si>
+    <t>Caster Wheels 5/8” </t>
+  </si>
+  <si>
+    <t>Sonar Mounts* </t>
+  </si>
+  <si>
+    <t>HC-SR04 Sonar * </t>
+  </si>
+  <si>
+    <t>IR Mounts* </t>
+  </si>
+  <si>
+    <t>Sharp IR Sensor* </t>
+  </si>
+  <si>
+    <t>LEDs* </t>
+  </si>
+  <si>
+    <t>Buzzer* </t>
+  </si>
+  <si>
+    <t>Slider Switch* </t>
+  </si>
+  <si>
+    <t>Photoresistor* </t>
+  </si>
+  <si>
+    <t>10kΩ resistor* </t>
+  </si>
+  <si>
+    <t>100Ω resistor* </t>
+  </si>
+  <si>
+    <t>Various Wires (Male-Male, Male-Female) </t>
+  </si>
+  <si>
+    <t>6mm panhead screws </t>
+  </si>
+  <si>
+    <t>8 mm panhead screws </t>
+  </si>
+  <si>
+    <t>25mm panhead screws </t>
+  </si>
+  <si>
+    <t>Phillips head screwdriver </t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Qty.</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Part ID#</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +162,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF2F5496"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,7 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -151,6 +214,19 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -467,196 +543,512 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA4E9AE-C5A9-4397-8E7C-B2931FC71F17}">
-  <dimension ref="B3:F24"/>
+  <dimension ref="A3:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:E24"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
+      <c r="C4" s="6">
+        <v>1</v>
       </c>
       <c r="D4" s="4">
         <v>7</v>
       </c>
       <c r="E4" s="4">
-        <f>D4*B4</f>
+        <f>D4*C4</f>
         <v>7</v>
       </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
       </c>
       <c r="D5" s="4">
         <v>1.1666000000000001</v>
       </c>
       <c r="E5" s="4">
-        <f>D5*B5</f>
-        <v>2.3332000000000002</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
+        <f t="shared" ref="E5:E6" si="0">D5*C5</f>
+        <v>1.1666000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4</v>
       </c>
       <c r="D6" s="4">
         <v>1.62</v>
       </c>
       <c r="E6" s="4">
-        <f>D6*B6</f>
-        <v>3.24</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
+        <f t="shared" si="0"/>
+        <v>6.48</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4">
+        <f>D7*C7</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
+      <c r="C8" s="6">
+        <v>1</v>
       </c>
       <c r="D8" s="4">
         <v>6.26</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" ref="E8:E13" si="0">D8*B8</f>
+        <f t="shared" ref="E8:E29" si="1">D8*C8</f>
         <v>6.26</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
+    </row>
+    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
+      <c r="C9" s="6">
+        <v>2</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6">
         <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="6">
+        <v>4</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1">
-        <f>SUM(E4:E13)</f>
-        <v>18.833199999999998</v>
-      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6">
+        <v>4</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6">
+        <v>20</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="6">
+        <v>2</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="6">
+        <v>8</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="6">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="4">
+        <f>D30*C30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="1">
+        <f>SUM(E4:E30)</f>
+        <v>20.906600000000001</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H48" s="7"/>
+      <c r="I48" s="8"/>
+    </row>
+    <row r="49" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H49" s="9"/>
+      <c r="I49" s="8"/>
+    </row>
+    <row r="50" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H50" s="9"/>
+      <c r="I50" s="8"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" xr:uid="{9DE8656A-6B97-403F-AD82-179BA58EF33A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>